<commit_message>
paper - still need to add PP
</commit_message>
<xml_diff>
--- a/Model/Example_Output_File/HPGe_Parameters.xlsx
+++ b/Model/Example_Output_File/HPGe_Parameters.xlsx
@@ -517,7 +517,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -729,37 +729,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -906,63 +880,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
@@ -970,12 +887,67 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1274,22 +1246,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.65">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="84"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="95"/>
       <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A2" s="28"/>
       <c r="B2" s="25"/>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="96" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="85"/>
+      <c r="D2" s="96"/>
       <c r="E2" s="26"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.65">
@@ -1357,7 +1329,7 @@
         <f t="shared" ref="D5:D20" si="1">B5+B5*0.1</f>
         <v>4.4219999999999997</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="91" t="s">
         <v>105</v>
       </c>
       <c r="I5" s="54" t="s">
@@ -1388,7 +1360,7 @@
         <f t="shared" si="1"/>
         <v>4.5650000000000004</v>
       </c>
-      <c r="E6" s="80"/>
+      <c r="E6" s="91"/>
       <c r="I6" s="54" t="s">
         <v>112</v>
       </c>
@@ -1417,7 +1389,7 @@
         <f t="shared" si="1"/>
         <v>0.14300000000000085</v>
       </c>
-      <c r="E7" s="80"/>
+      <c r="E7" s="91"/>
       <c r="I7" s="57" t="s">
         <v>113</v>
       </c>
@@ -1446,7 +1418,7 @@
         <f t="shared" si="1"/>
         <v>9.152000000000001</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="91" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="48" t="s">
@@ -1477,7 +1449,7 @@
         <f t="shared" si="1"/>
         <v>9.2949999999999999</v>
       </c>
-      <c r="E9" s="80"/>
+      <c r="E9" s="91"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A10" s="42" t="s">
@@ -1494,7 +1466,7 @@
         <f t="shared" si="1"/>
         <v>0.14300000000000085</v>
       </c>
-      <c r="E10" s="80"/>
+      <c r="E10" s="91"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A11" s="51" t="s">
@@ -1511,7 +1483,7 @@
         <f t="shared" si="1"/>
         <v>0.495</v>
       </c>
-      <c r="E11" s="80" t="s">
+      <c r="E11" s="91" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1530,7 +1502,7 @@
         <f t="shared" si="1"/>
         <v>3.2999999999971942E-5</v>
       </c>
-      <c r="E12" s="80"/>
+      <c r="E12" s="91"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A13" s="33" t="s">
@@ -1547,7 +1519,7 @@
         <f t="shared" si="1"/>
         <v>7.6449999999999996</v>
       </c>
-      <c r="E13" s="80" t="s">
+      <c r="E13" s="91" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1566,7 +1538,7 @@
         <f t="shared" si="1"/>
         <v>3.3000000000704687E-5</v>
       </c>
-      <c r="E14" s="80"/>
+      <c r="E14" s="91"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.65">
       <c r="A15" s="33" t="s">
@@ -1671,57 +1643,57 @@
       <c r="E20" s="32"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.65">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="92"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.65">
-      <c r="A22" s="81"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
+      <c r="A22" s="92"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="92"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.65">
-      <c r="A23" s="81"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
+      <c r="A23" s="92"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="92"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.65">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.65">
-      <c r="A25" s="81"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
+      <c r="A25" s="92"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.65">
-      <c r="A26" s="81"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
+      <c r="A26" s="92"/>
+      <c r="B26" s="92"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="92"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.65">
-      <c r="A27" s="81"/>
-      <c r="B27" s="81"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
+      <c r="A27" s="92"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1776,13 +1748,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A2" s="86">
+      <c r="A2" s="97">
         <v>2</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="92">
+      <c r="C2" s="103">
         <v>8.41</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1796,9 +1768,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A3" s="87"/>
-      <c r="B3" s="90"/>
-      <c r="C3" s="93"/>
+      <c r="A3" s="98"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="104"/>
       <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
@@ -1810,9 +1782,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A4" s="88"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="94"/>
+      <c r="A4" s="99"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="105"/>
       <c r="D4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1944,13 +1916,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A11" s="86">
+      <c r="A11" s="97">
         <v>9</v>
       </c>
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="92">
+      <c r="C11" s="103">
         <v>1.42</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1964,9 +1936,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A12" s="87"/>
-      <c r="B12" s="90"/>
-      <c r="C12" s="93"/>
+      <c r="A12" s="98"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="104"/>
       <c r="D12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1978,9 +1950,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A13" s="87"/>
-      <c r="B13" s="90"/>
-      <c r="C13" s="93"/>
+      <c r="A13" s="98"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="104"/>
       <c r="D13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1992,9 +1964,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A14" s="88"/>
-      <c r="B14" s="91"/>
-      <c r="C14" s="94"/>
+      <c r="A14" s="99"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="105"/>
       <c r="D14" s="4" t="s">
         <v>39</v>
       </c>
@@ -2006,13 +1978,13 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A15" s="86">
+      <c r="A15" s="97">
         <v>10</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="92">
+      <c r="C15" s="103">
         <v>1.225E-3</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -2026,9 +1998,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A16" s="87"/>
-      <c r="B16" s="90"/>
-      <c r="C16" s="93"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="104"/>
       <c r="D16" s="3" t="s">
         <v>39</v>
       </c>
@@ -2040,9 +2012,9 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A17" s="88"/>
-      <c r="B17" s="91"/>
-      <c r="C17" s="94"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="102"/>
+      <c r="C17" s="105"/>
       <c r="D17" s="4" t="s">
         <v>41</v>
       </c>
@@ -2074,13 +2046,13 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A19" s="86">
+      <c r="A19" s="97">
         <v>12</v>
       </c>
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="92">
+      <c r="C19" s="103">
         <v>1.38</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -2094,9 +2066,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.65">
-      <c r="A20" s="87"/>
-      <c r="B20" s="90"/>
-      <c r="C20" s="93"/>
+      <c r="A20" s="98"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="104"/>
       <c r="D20" s="3" t="s">
         <v>37</v>
       </c>
@@ -2108,9 +2080,9 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A21" s="88"/>
-      <c r="B21" s="91"/>
-      <c r="C21" s="94"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="105"/>
       <c r="D21" s="4" t="s">
         <v>39</v>
       </c>
@@ -2134,18 +2106,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="C19:C21"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2167,15 +2139,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="97"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="108"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A2" s="1" t="s">
@@ -2284,15 +2256,15 @@
       <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A8" s="95" t="s">
+      <c r="A8" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="97"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="107"/>
+      <c r="G8" s="108"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A9" s="1" t="s">
@@ -2433,15 +2405,15 @@
       <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A17" s="95" t="s">
+      <c r="A17" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="96"/>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="97"/>
+      <c r="B17" s="107"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="108"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A18" s="1" t="s">
@@ -2508,15 +2480,15 @@
       <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="106" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="96"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="97"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="107"/>
+      <c r="D22" s="107"/>
+      <c r="E22" s="107"/>
+      <c r="F22" s="107"/>
+      <c r="G22" s="108"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A23" s="1" t="s">
@@ -2683,15 +2655,15 @@
       <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A32" s="95" t="s">
+      <c r="A32" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="96"/>
-      <c r="C32" s="96"/>
-      <c r="D32" s="96"/>
-      <c r="E32" s="96"/>
-      <c r="F32" s="96"/>
-      <c r="G32" s="97"/>
+      <c r="B32" s="107"/>
+      <c r="C32" s="107"/>
+      <c r="D32" s="107"/>
+      <c r="E32" s="107"/>
+      <c r="F32" s="107"/>
+      <c r="G32" s="108"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A33" s="1" t="s">
@@ -2793,15 +2765,15 @@
       <c r="G38" s="23"/>
     </row>
     <row r="39" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A39" s="95" t="s">
+      <c r="A39" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="96"/>
-      <c r="C39" s="96"/>
-      <c r="D39" s="96"/>
-      <c r="E39" s="96"/>
-      <c r="F39" s="96"/>
-      <c r="G39" s="97"/>
+      <c r="B39" s="107"/>
+      <c r="C39" s="107"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="107"/>
+      <c r="F39" s="107"/>
+      <c r="G39" s="108"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A40" s="1" t="s">
@@ -3074,8 +3046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:M12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -3092,12 +3064,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.65">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
@@ -3113,10 +3085,10 @@
     <row r="2" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A2" s="28"/>
       <c r="B2" s="25"/>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="96" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="85"/>
+      <c r="D2" s="96"/>
     </row>
     <row r="3" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A3" s="30" t="s">
@@ -3185,38 +3157,38 @@
       <c r="E4" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="99">
+      <c r="F4" s="80">
         <v>12.35</v>
       </c>
-      <c r="G4" s="102">
+      <c r="G4" s="83">
         <f>F24-(F4-G24)</f>
         <v>0.73899333000000134</v>
       </c>
-      <c r="H4" s="99">
+      <c r="H4" s="80">
         <v>12.35</v>
       </c>
-      <c r="I4" s="104">
+      <c r="I4" s="85">
         <f>F24-(H4-G24)</f>
         <v>0.73899333000000134</v>
       </c>
-      <c r="J4" s="99">
+      <c r="J4" s="80">
         <v>12.35</v>
       </c>
-      <c r="K4" s="108">
+      <c r="K4" s="87">
         <f>F24-(J4-G24)</f>
         <v>0.73899333000000134</v>
       </c>
-      <c r="L4" s="109">
+      <c r="L4" s="88">
         <v>12.35</v>
       </c>
-      <c r="M4" s="108">
+      <c r="M4" s="87">
         <f>F24-(L4-G24)</f>
         <v>0.73899333000000134</v>
       </c>
-      <c r="N4" s="109">
+      <c r="N4" s="88">
         <v>12.35</v>
       </c>
-      <c r="O4" s="110">
+      <c r="O4" s="89">
         <f>F24-(N4-G24)</f>
         <v>0.73899333000000134</v>
       </c>
@@ -3249,38 +3221,38 @@
       <c r="E5" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="99">
+      <c r="F5" s="80">
         <v>3.92</v>
       </c>
-      <c r="G5" s="102">
+      <c r="G5" s="83">
         <f>F25-(F5-G25)</f>
         <v>0.23000000000000043</v>
       </c>
-      <c r="H5" s="99">
+      <c r="H5" s="80">
         <v>3.92</v>
       </c>
-      <c r="I5" s="104">
+      <c r="I5" s="85">
         <f t="shared" ref="I5:I6" si="1">F25-(H5-G25)</f>
         <v>0.23000000000000043</v>
       </c>
-      <c r="J5" s="99">
+      <c r="J5" s="80">
         <v>3.92</v>
       </c>
-      <c r="K5" s="108">
+      <c r="K5" s="87">
         <f t="shared" ref="K5:K6" si="2">F25-(J5-G25)</f>
         <v>0.23000000000000043</v>
       </c>
-      <c r="L5" s="109">
+      <c r="L5" s="88">
         <v>2.8</v>
       </c>
-      <c r="M5" s="108">
+      <c r="M5" s="87">
         <f t="shared" ref="M5:M6" si="3">F25-(L5-G25)</f>
         <v>1.3500000000000005</v>
       </c>
-      <c r="N5" s="109">
+      <c r="N5" s="88">
         <v>3.92</v>
       </c>
-      <c r="O5" s="110">
+      <c r="O5" s="89">
         <f t="shared" ref="O5:O6" si="4">F25-(N5-G25)</f>
         <v>0.23000000000000043</v>
       </c>
@@ -3315,38 +3287,38 @@
       <c r="E6" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="F6" s="99">
+      <c r="F6" s="80">
         <v>5.296220666</v>
       </c>
-      <c r="G6" s="102">
+      <c r="G6" s="83">
         <f>F26-(F6-G26)</f>
         <v>7.6627726640000002</v>
       </c>
-      <c r="H6" s="99">
+      <c r="H6" s="80">
         <v>5.4839993329999999</v>
       </c>
-      <c r="I6" s="104">
+      <c r="I6" s="85">
         <f t="shared" si="1"/>
         <v>7.4749939970000003</v>
       </c>
-      <c r="J6" s="99">
+      <c r="J6" s="80">
         <v>5.4839993329999999</v>
       </c>
-      <c r="K6" s="108">
+      <c r="K6" s="87">
         <f t="shared" si="2"/>
         <v>7.4749939970000003</v>
       </c>
-      <c r="L6" s="109">
+      <c r="L6" s="88">
         <v>5.4839993329999999</v>
       </c>
-      <c r="M6" s="108">
+      <c r="M6" s="87">
         <f t="shared" si="3"/>
         <v>7.4749939970000003</v>
       </c>
-      <c r="N6" s="109">
+      <c r="N6" s="88">
         <v>5.4839993329999999</v>
       </c>
-      <c r="O6" s="110">
+      <c r="O6" s="89">
         <f t="shared" si="4"/>
         <v>7.4749939970000003</v>
       </c>
@@ -3381,38 +3353,38 @@
       <c r="E7" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="99">
+      <c r="F7" s="80">
         <v>13.2</v>
       </c>
-      <c r="G7" s="102">
+      <c r="G7" s="83">
         <f>F27+(F7-G27)</f>
         <v>0.1101599999999987</v>
       </c>
-      <c r="H7" s="99">
+      <c r="H7" s="80">
         <v>13.2</v>
       </c>
-      <c r="I7" s="104">
+      <c r="I7" s="85">
         <f>F27+(H7-G27)</f>
         <v>0.1101599999999987</v>
       </c>
-      <c r="J7" s="99">
+      <c r="J7" s="80">
         <v>13.2</v>
       </c>
-      <c r="K7" s="104">
+      <c r="K7" s="85">
         <f>F27+ABS(J7-G27)</f>
         <v>0.1101599999999987</v>
       </c>
-      <c r="L7" s="109">
+      <c r="L7" s="88">
         <v>13.147500000000001</v>
       </c>
-      <c r="M7" s="104">
+      <c r="M7" s="85">
         <f>F27+ABS(L7-G27)</f>
         <v>5.7660000000000267E-2</v>
       </c>
-      <c r="N7" s="109">
+      <c r="N7" s="88">
         <v>13.2</v>
       </c>
-      <c r="O7" s="111">
+      <c r="O7" s="90">
         <f>F27+ABS(N7-G27)</f>
         <v>0.1101599999999987</v>
       </c>
@@ -3447,38 +3419,38 @@
       <c r="E8" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="99">
+      <c r="F8" s="80">
         <v>11.58912333</v>
       </c>
-      <c r="G8" s="102">
+      <c r="G8" s="83">
         <f>F28-(G28-F8)</f>
         <v>1.2999999999974143E-4</v>
       </c>
-      <c r="H8" s="99">
+      <c r="H8" s="80">
         <v>11.589054257800001</v>
       </c>
-      <c r="I8" s="104">
+      <c r="I8" s="85">
         <f>F28+(H8-G28)</f>
         <v>6.0927800000998289E-5</v>
       </c>
-      <c r="J8" s="99">
+      <c r="J8" s="80">
         <v>11.589054257800001</v>
       </c>
-      <c r="K8" s="104">
+      <c r="K8" s="85">
         <f>F28+ABS(J8-G28)</f>
         <v>6.0927800000998289E-5</v>
       </c>
-      <c r="L8" s="109">
+      <c r="L8" s="88">
         <v>11.5890957011</v>
       </c>
-      <c r="M8" s="104">
+      <c r="M8" s="85">
         <f>F28+ABS(L8-G28)</f>
         <v>1.0237109999988725E-4</v>
       </c>
-      <c r="N8" s="109">
+      <c r="N8" s="88">
         <v>11.589054257800001</v>
       </c>
-      <c r="O8" s="111">
+      <c r="O8" s="90">
         <f>F28+ABS(N8-G28)</f>
         <v>6.0927800000998289E-5</v>
       </c>
@@ -3513,38 +3485,38 @@
       <c r="E9" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="F9" s="99">
+      <c r="F9" s="80">
         <v>0.45001999999999998</v>
       </c>
-      <c r="G9" s="102">
+      <c r="G9" s="83">
         <f>F29-(G29-F9)</f>
         <v>1.9999999999964491E-5</v>
       </c>
-      <c r="H9" s="99">
+      <c r="H9" s="80">
         <v>0.45006000000000002</v>
       </c>
-      <c r="I9" s="104">
+      <c r="I9" s="85">
         <f>F29-(G29-H9)</f>
         <v>6.0000000000004494E-5</v>
       </c>
-      <c r="J9" s="99">
+      <c r="J9" s="80">
         <v>0.45007000000000003</v>
       </c>
-      <c r="K9" s="104">
+      <c r="K9" s="85">
         <f>F29-(G29-J9)</f>
         <v>7.0000000000014495E-5</v>
       </c>
-      <c r="L9" s="109">
+      <c r="L9" s="88">
         <v>0.45100000000000001</v>
       </c>
-      <c r="M9" s="104">
+      <c r="M9" s="85">
         <f>F29-(G29-L9)</f>
         <v>1.0000000000000009E-3</v>
       </c>
-      <c r="N9" s="109">
+      <c r="N9" s="88">
         <v>0.45007000000000003</v>
       </c>
-      <c r="O9" s="111">
+      <c r="O9" s="90">
         <f>F29-(G29-N9)</f>
         <v>7.0000000000014495E-5</v>
       </c>
@@ -3567,38 +3539,38 @@
       <c r="E10" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="F10" s="99">
+      <c r="F10" s="80">
         <v>13.35</v>
       </c>
-      <c r="G10" s="102">
+      <c r="G10" s="83">
         <f>F30-(F10-G30)</f>
         <v>0.24999999999999964</v>
       </c>
-      <c r="H10" s="99">
+      <c r="H10" s="80">
         <v>13.35</v>
       </c>
-      <c r="I10" s="104">
+      <c r="I10" s="85">
         <f>F30-(H10-G30)</f>
         <v>0.24999999999999964</v>
       </c>
-      <c r="J10" s="99">
+      <c r="J10" s="80">
         <v>13.35</v>
       </c>
-      <c r="K10" s="104">
+      <c r="K10" s="85">
         <f>F30-(J10-G30)</f>
         <v>0.24999999999999964</v>
       </c>
-      <c r="L10" s="109">
+      <c r="L10" s="88">
         <v>13.55</v>
       </c>
-      <c r="M10" s="104">
+      <c r="M10" s="85">
         <f>F30-(L10-G30)</f>
         <v>4.9999999999998573E-2</v>
       </c>
-      <c r="N10" s="109">
+      <c r="N10" s="88">
         <v>13.35</v>
       </c>
-      <c r="O10" s="111">
+      <c r="O10" s="90">
         <f>F30-(N10-G30)</f>
         <v>0.24999999999999964</v>
       </c>
@@ -3621,39 +3593,39 @@
       <c r="E11" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="F11" s="99">
+      <c r="F11" s="80">
         <v>4.7</v>
       </c>
-      <c r="G11" s="102">
+      <c r="G11" s="83">
         <f>F31-(F11-G31)</f>
         <v>4.9999999999999462E-2</v>
       </c>
-      <c r="H11" s="99">
+      <c r="H11" s="80">
         <v>4.7</v>
       </c>
-      <c r="I11" s="104">
+      <c r="I11" s="85">
         <f>F31-(H11-G31)</f>
         <v>4.9999999999999462E-2</v>
       </c>
-      <c r="J11" s="99">
+      <c r="J11" s="80">
         <v>4.7</v>
       </c>
-      <c r="K11" s="104">
-        <f t="shared" ref="K11:K12" si="6">F31-(J11-G31)</f>
+      <c r="K11" s="85">
+        <f t="shared" ref="K11" si="6">F31-(J11-G31)</f>
         <v>4.9999999999999462E-2</v>
       </c>
-      <c r="L11" s="109">
+      <c r="L11" s="88">
         <v>4.4800000000000004</v>
       </c>
-      <c r="M11" s="104">
-        <f t="shared" ref="M11:M12" si="7">F31-(L11-G31)</f>
+      <c r="M11" s="85">
+        <f t="shared" ref="M11" si="7">F31-(L11-G31)</f>
         <v>0.26999999999999924</v>
       </c>
-      <c r="N11" s="109">
+      <c r="N11" s="88">
         <v>4.5</v>
       </c>
-      <c r="O11" s="111">
-        <f t="shared" ref="O11:O12" si="8">F31-(N11-G31)</f>
+      <c r="O11" s="90">
+        <f t="shared" ref="O11" si="8">F31-(N11-G31)</f>
         <v>0.24999999999999964</v>
       </c>
     </row>
@@ -3675,43 +3647,43 @@
       <c r="E12" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="F12" s="100">
+      <c r="F12" s="81">
         <v>5.32</v>
       </c>
-      <c r="G12" s="103">
+      <c r="G12" s="84">
         <f>F32-(F12-G32)</f>
         <v>5.32</v>
       </c>
-      <c r="H12" s="101">
+      <c r="H12" s="82">
         <v>5.32</v>
       </c>
-      <c r="I12" s="105">
+      <c r="I12" s="86">
         <f>F32-(H12-G32)</f>
         <v>5.32</v>
       </c>
-      <c r="J12" s="99">
+      <c r="J12" s="80">
         <v>5.35</v>
       </c>
-      <c r="K12" s="104">
+      <c r="K12" s="85">
         <f>J12</f>
         <v>5.35</v>
       </c>
-      <c r="L12" s="109">
+      <c r="L12" s="88">
         <v>5.32</v>
       </c>
-      <c r="M12" s="104">
+      <c r="M12" s="85">
         <f>L12</f>
         <v>5.32</v>
       </c>
-      <c r="N12" s="109">
+      <c r="N12" s="88">
         <v>5.3425000000000002</v>
       </c>
-      <c r="O12" s="111">
+      <c r="O12" s="90">
         <f>N12</f>
         <v>5.3425000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A13" s="33" t="s">
         <v>93</v>
       </c>
@@ -3733,14 +3705,19 @@
       <c r="G13" s="26"/>
       <c r="H13" s="28"/>
       <c r="I13" s="26"/>
-      <c r="J13" s="106"/>
-      <c r="K13" s="107"/>
+      <c r="J13" s="80">
+        <v>12.1136363636</v>
+      </c>
+      <c r="K13" s="87">
+        <f>F24-(J13-G24)</f>
+        <v>0.97535696640000147</v>
+      </c>
       <c r="L13" s="71"/>
       <c r="M13" s="72"/>
       <c r="N13" s="71"/>
       <c r="O13" s="72"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:21" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A14" s="63" t="s">
         <v>94</v>
       </c>
@@ -3762,8 +3739,13 @@
       <c r="G14" s="26"/>
       <c r="H14" s="28"/>
       <c r="I14" s="26"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="26"/>
+      <c r="J14" s="80">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="K14" s="87">
+        <f>F25-(J14-G25)</f>
+        <v>0.13000000000000078</v>
+      </c>
       <c r="L14" s="28"/>
       <c r="M14" s="26"/>
       <c r="N14" s="28"/>
@@ -3791,8 +3773,13 @@
       <c r="G15" s="26"/>
       <c r="H15" s="28"/>
       <c r="I15" s="26"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="26"/>
+      <c r="J15" s="80">
+        <v>4.3573273309999996</v>
+      </c>
+      <c r="K15" s="87">
+        <f>F26-(J15-G26)</f>
+        <v>8.6016659990000015</v>
+      </c>
       <c r="L15" s="28"/>
       <c r="M15" s="26"/>
       <c r="N15" s="28"/>
@@ -3820,8 +3807,13 @@
       <c r="G16" s="26"/>
       <c r="H16" s="28"/>
       <c r="I16" s="26"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="26"/>
+      <c r="J16" s="80">
+        <v>13.22</v>
+      </c>
+      <c r="K16" s="85">
+        <f>F27+ABS(J16-G27)</f>
+        <v>0.13016000000000005</v>
+      </c>
       <c r="L16" s="28"/>
       <c r="M16" s="26"/>
       <c r="N16" s="28"/>
@@ -3849,8 +3841,13 @@
       <c r="G17" s="26"/>
       <c r="H17" s="28"/>
       <c r="I17" s="26"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="26"/>
+      <c r="J17" s="80">
+        <v>11.5894995556</v>
+      </c>
+      <c r="K17" s="85">
+        <f>F28+ABS(J17-G28)</f>
+        <v>5.062255999999099E-4</v>
+      </c>
       <c r="L17" s="28"/>
       <c r="M17" s="26"/>
       <c r="N17" s="28"/>
@@ -3878,8 +3875,13 @@
       <c r="G18" s="26"/>
       <c r="H18" s="28"/>
       <c r="I18" s="26"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="26"/>
+      <c r="J18" s="80">
+        <v>0.45005000000000001</v>
+      </c>
+      <c r="K18" s="85">
+        <f>F29-(G29-J18)</f>
+        <v>4.9999999999994493E-5</v>
+      </c>
       <c r="L18" s="28"/>
       <c r="M18" s="26"/>
       <c r="N18" s="28"/>
@@ -3907,8 +3909,13 @@
       <c r="G19" s="26"/>
       <c r="H19" s="28"/>
       <c r="I19" s="26"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="26"/>
+      <c r="J19" s="80">
+        <v>13.416666666699999</v>
+      </c>
+      <c r="K19" s="85">
+        <f>F30-(J19-G30)</f>
+        <v>0.18333333329999987</v>
+      </c>
       <c r="L19" s="28"/>
       <c r="M19" s="26"/>
       <c r="N19" s="28"/>
@@ -3936,20 +3943,25 @@
       <c r="G20" s="26"/>
       <c r="H20" s="28"/>
       <c r="I20" s="26"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="26"/>
+      <c r="J20" s="80">
+        <v>4.5</v>
+      </c>
+      <c r="K20" s="85">
+        <f>F31-(J20-G31)</f>
+        <v>0.24999999999999964</v>
+      </c>
       <c r="L20" s="28"/>
       <c r="M20" s="26"/>
       <c r="N20" s="28"/>
       <c r="O20" s="26"/>
     </row>
     <row r="21" spans="1:15" ht="14.5" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="98"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="109"/>
       <c r="E21" s="78" t="s">
         <v>129</v>
       </c>
@@ -3957,18 +3969,23 @@
       <c r="G21" s="74"/>
       <c r="H21" s="73"/>
       <c r="I21" s="74"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="74"/>
+      <c r="J21" s="80">
+        <v>5.35</v>
+      </c>
+      <c r="K21" s="85">
+        <f>J21</f>
+        <v>5.35</v>
+      </c>
       <c r="L21" s="73"/>
       <c r="M21" s="74"/>
       <c r="N21" s="73"/>
       <c r="O21" s="74"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A22" s="81"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="98"/>
+      <c r="A22" s="92"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="109"/>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
@@ -3980,10 +3997,10 @@
       <c r="M22" s="25"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A23" s="81"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
+      <c r="A23" s="92"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
       <c r="F23" t="s">
         <v>136</v>
       </c>
@@ -4004,12 +4021,12 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
       <c r="E24" t="s">
         <v>126</v>
       </c>
@@ -4047,10 +4064,10 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A25" s="81"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
+      <c r="A25" s="92"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
       <c r="E25" t="s">
         <v>128</v>
       </c>
@@ -4088,10 +4105,10 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A26" s="81"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
+      <c r="A26" s="92"/>
+      <c r="B26" s="92"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="92"/>
       <c r="E26" t="s">
         <v>127</v>
       </c>
@@ -4129,10 +4146,10 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.65">
-      <c r="A27" s="81"/>
-      <c r="B27" s="81"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
+      <c r="A27" s="92"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="92"/>
       <c r="E27" t="s">
         <v>132</v>
       </c>

</xml_diff>